<commit_message>
Preliminary BOC form skeleton
</commit_message>
<xml_diff>
--- a/boc.xlsx
+++ b/boc.xlsx
@@ -339,12 +339,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -352,6 +346,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -809,8 +809,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="X10" sqref="X10"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -839,28 +839,28 @@
       </c>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="5" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
+      <c r="A3" s="6"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
     </row>
     <row r="6" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -868,99 +868,99 @@
       </c>
     </row>
     <row r="7" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="F7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G7" s="4" t="s">
+      <c r="G7" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H7" s="4" t="s">
+      <c r="H7" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I7" s="1" t="s">
+      <c r="I7" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="J7" s="1" t="s">
+      <c r="J7" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="K7" s="1" t="s">
+      <c r="K7" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="L7" s="1" t="s">
+      <c r="L7" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="M7" s="1" t="s">
+      <c r="M7" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="N7" s="1" t="s">
+      <c r="N7" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="O7" s="1" t="s">
+      <c r="O7" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="P7" s="1" t="s">
+      <c r="P7" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="Q7" s="1" t="s">
+      <c r="Q7" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="R7" s="1" t="s">
+      <c r="R7" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="S7" s="1" t="s">
+      <c r="S7" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="T7" s="1" t="s">
+      <c r="T7" s="5" t="s">
         <v>24</v>
       </c>
       <c r="U7" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="V7" s="1" t="s">
+      <c r="V7" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="W7" s="1" t="s">
+      <c r="W7" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="X7" s="1" t="s">
+      <c r="X7" s="5" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:24" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
-      <c r="L8" s="2"/>
-      <c r="M8" s="2"/>
-      <c r="N8" s="2"/>
-      <c r="O8" s="2"/>
-      <c r="P8" s="2"/>
-      <c r="Q8" s="2"/>
-      <c r="R8" s="2"/>
-      <c r="S8" s="2"/>
-      <c r="T8" s="2"/>
+      <c r="A8" s="6"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="6"/>
+      <c r="L8" s="6"/>
+      <c r="M8" s="6"/>
+      <c r="N8" s="6"/>
+      <c r="O8" s="6"/>
+      <c r="P8" s="6"/>
+      <c r="Q8" s="6"/>
+      <c r="R8" s="6"/>
+      <c r="S8" s="6"/>
+      <c r="T8" s="6"/>
       <c r="U8" s="8"/>
-      <c r="V8" s="2"/>
-      <c r="W8" s="2"/>
-      <c r="X8" s="2"/>
+      <c r="V8" s="6"/>
+      <c r="W8" s="6"/>
+      <c r="X8" s="6"/>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -1051,7 +1051,7 @@
       </c>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="4" t="s">
         <v>36</v>
       </c>
       <c r="P11" t="s">
@@ -1068,7 +1068,7 @@
       </c>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="4" t="s">
         <v>38</v>
       </c>
       <c r="Q12" t="s">
@@ -1082,27 +1082,12 @@
       </c>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="4" t="s">
         <v>40</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="T7:T8"/>
-    <mergeCell ref="U7:U8"/>
-    <mergeCell ref="V7:V8"/>
-    <mergeCell ref="W7:W8"/>
-    <mergeCell ref="X7:X8"/>
-    <mergeCell ref="O7:O8"/>
-    <mergeCell ref="P7:P8"/>
-    <mergeCell ref="Q7:Q8"/>
-    <mergeCell ref="R7:R8"/>
-    <mergeCell ref="S7:S8"/>
-    <mergeCell ref="I7:I8"/>
-    <mergeCell ref="J7:J8"/>
-    <mergeCell ref="K7:K8"/>
-    <mergeCell ref="L7:L8"/>
-    <mergeCell ref="M7:M8"/>
     <mergeCell ref="N7:N8"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="A2:A3"/>
@@ -1111,6 +1096,21 @@
     <mergeCell ref="E2:E3"/>
     <mergeCell ref="A7:A8"/>
     <mergeCell ref="C7:C8"/>
+    <mergeCell ref="I7:I8"/>
+    <mergeCell ref="J7:J8"/>
+    <mergeCell ref="K7:K8"/>
+    <mergeCell ref="L7:L8"/>
+    <mergeCell ref="M7:M8"/>
+    <mergeCell ref="O7:O8"/>
+    <mergeCell ref="P7:P8"/>
+    <mergeCell ref="Q7:Q8"/>
+    <mergeCell ref="R7:R8"/>
+    <mergeCell ref="S7:S8"/>
+    <mergeCell ref="T7:T8"/>
+    <mergeCell ref="U7:U8"/>
+    <mergeCell ref="V7:V8"/>
+    <mergeCell ref="W7:W8"/>
+    <mergeCell ref="X7:X8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>